<commit_message>
add model, add tensorboard-keras
</commit_message>
<xml_diff>
--- a/参数影响.xlsx
+++ b/参数影响.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>batch_size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>GTX1062</t>
+  </si>
+  <si>
+    <t>model_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lstm_epochs10_dropout0.3_v1.h5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lstm_epochs30_dropout0.3_v1.h5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -216,7 +228,10 @@
     <cellStyle name="好" xfId="1" builtinId="26"/>
     <cellStyle name="适中" xfId="3" builtinId="28"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -282,19 +297,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:J9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J9"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="epochs" dataDxfId="9"/>
-    <tableColumn id="2" name="time_steps" dataDxfId="8"/>
-    <tableColumn id="3" name="input_size" dataDxfId="7"/>
-    <tableColumn id="4" name="output_size" dataDxfId="6"/>
-    <tableColumn id="5" name="batch_size" dataDxfId="5"/>
-    <tableColumn id="11" name="drop_out" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K9"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="epochs" dataDxfId="10"/>
+    <tableColumn id="2" name="time_steps" dataDxfId="9"/>
+    <tableColumn id="3" name="input_size" dataDxfId="8"/>
+    <tableColumn id="4" name="output_size" dataDxfId="7"/>
+    <tableColumn id="5" name="batch_size" dataDxfId="6"/>
+    <tableColumn id="11" name="drop_out" dataDxfId="5"/>
     <tableColumn id="6" name="GPU" dataDxfId="4"/>
     <tableColumn id="7" name="MAE" dataDxfId="3"/>
     <tableColumn id="8" name="RMSE" dataDxfId="2"/>
     <tableColumn id="9" name="MAPE" dataDxfId="1"/>
+    <tableColumn id="10" name="model_name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -579,9 +595,10 @@
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="9" width="11.5546875" customWidth="1"/>
     <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="11" max="11" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -612,8 +629,11 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>10</v>
       </c>
@@ -644,8 +664,9 @@
       <c r="J2" s="3">
         <v>0.13539999999999999</v>
       </c>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>20</v>
       </c>
@@ -676,8 +697,9 @@
       <c r="J3" s="3">
         <v>0.13819999999999999</v>
       </c>
+      <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>30</v>
       </c>
@@ -708,8 +730,9 @@
       <c r="J4" s="3">
         <v>0.1343</v>
       </c>
+      <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>40</v>
       </c>
@@ -740,8 +763,9 @@
       <c r="J5" s="6">
         <v>0.1211</v>
       </c>
+      <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>10</v>
       </c>
@@ -772,8 +796,11 @@
       <c r="J6" s="3">
         <v>0.124</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>20</v>
       </c>
@@ -798,8 +825,9 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>30</v>
       </c>
@@ -830,8 +858,11 @@
       <c r="J8" s="3">
         <v>0.1071</v>
       </c>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -842,6 +873,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>